<commit_message>
DF, init DV and ETL archive
</commit_message>
<xml_diff>
--- a/metadata/definition/meta_hsat_mapping.xlsx
+++ b/metadata/definition/meta_hsat_mapping.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\golddwh\metadata\definition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B282F146-88F7-40F9-8181-28DF098E1363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED3BCF99-743C-40A3-9803-FC6A08ECC81D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" tabRatio="513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="23235" windowHeight="13935" tabRatio="513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hsat" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -804,13 +805,7 @@
   <autoFilter ref="A1:V96" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="hsat_account"/>
-        <filter val="hsat_address"/>
-        <filter val="hsat_card"/>
-        <filter val="hsat_card_merchant"/>
         <filter val="hsat_customer"/>
-        <filter val="hsat_partner"/>
-        <filter val="hsat_user"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1166,8 +1161,8 @@
   <dimension ref="A1:V119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1174,7 @@
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
@@ -1264,7 +1259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -1320,7 +1315,7 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -1370,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1426,7 +1421,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1482,7 +1477,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2188,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -2244,7 +2239,7 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2294,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -2344,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -2394,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -2444,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -2847,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -2903,7 +2898,7 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -2953,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -3003,7 +2998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -3053,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -3103,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -3159,7 +3154,7 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -3209,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -3259,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -3309,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -3359,7 +3354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -3409,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>26</v>
       </c>
@@ -3459,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
@@ -3509,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
@@ -3559,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>26</v>
       </c>
@@ -3609,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -3659,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -3709,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>26</v>
       </c>
@@ -3809,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>26</v>
       </c>
@@ -3859,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>26</v>
       </c>
@@ -3909,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>26</v>
       </c>
@@ -3959,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>26</v>
       </c>
@@ -4009,7 +4004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>